<commit_message>
Adicionando hiperlinks - finalização
</commit_message>
<xml_diff>
--- a/módulo 04/aula-hiperlinks.xlsx
+++ b/módulo 04/aula-hiperlinks.xlsx
@@ -5,14 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nelio\Google Drive\Cursos online\Curso_Excel\04 Mais tópicos de edição e formatação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\Curso Excel do básico ao avançado\módulo 04\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="8130"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10125" windowHeight="6780" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Menu" sheetId="1" r:id="rId1"/>
+    <sheet name="Lançamentos" sheetId="2" r:id="rId2"/>
+    <sheet name="Relatório" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -21,6 +23,14 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+  <si>
+    <t>Inserir hiperlink no mesmo doc: clica no objeto desejado/inserir/hiperlink/colocar neste documento/escolhe a planilha desejada</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -228,9 +238,10 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="8" name="Retângulo: Único Canto Recortado 7">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{68D92666-11B7-401A-B465-5FF5EE91444B}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68D92666-11B7-401A-B465-5FF5EE91444B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -309,7 +320,7 @@
         <xdr:cNvPr id="16" name="Imagem 15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8DD455D8-DD2E-4E47-A793-02EFDF9CAC96}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DD455D8-DD2E-4E47-A793-02EFDF9CAC96}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -318,7 +329,7 @@
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill rotWithShape="1">
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
         <a:srcRect t="4111" b="8450"/>
         <a:stretch/>
       </xdr:blipFill>
@@ -352,7 +363,7 @@
         <xdr:cNvPr id="17" name="CaixaDeTexto 16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{88F505DC-0525-4B37-B8DC-24B423530C24}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88F505DC-0525-4B37-B8DC-24B423530C24}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -435,9 +446,10 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="7" name="Retângulo: Único Canto Recortado 6">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{61A5EA32-C5C9-47A5-A9FE-68ABE8608E4C}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61A5EA32-C5C9-47A5-A9FE-68ABE8608E4C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -512,9 +524,10 @@
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
         <xdr:cNvPr id="11" name="Retângulo: Único Canto Recortado 10">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8F6DEA5C-FE02-4F70-AC4E-521F970DE373}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F6DEA5C-FE02-4F70-AC4E-521F970DE373}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -531,6 +544,742 @@
           </a:avLst>
         </a:prstGeom>
         <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="72000" rIns="36000" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1000">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+            </a:rPr>
+            <a:t>RELATÓRIOS</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>560475</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>60525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo: Único Canto Recortado 7">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68D92666-11B7-401A-B465-5FF5EE91444B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="257175" y="514350"/>
+          <a:ext cx="1332000" cy="432000"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip1Rect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 47535"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="72000" rIns="36000" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1000">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+            </a:rPr>
+            <a:t>MENU</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>155113</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DD455D8-DD2E-4E47-A793-02EFDF9CAC96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect t="4111" b="8450"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4286250" y="1162050"/>
+          <a:ext cx="3133725" cy="2784013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>314850</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>504000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="CaixaDeTexto 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88F505DC-0525-4B37-B8DC-24B423530C24}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="0"/>
+          <a:ext cx="3420000" cy="504000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1500">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>GERENCIADOR</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1500" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> DE ESTOQUES</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1500">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>350925</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>60525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Retângulo: Único Canto Recortado 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61A5EA32-C5C9-47A5-A9FE-68ABE8608E4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1609725" y="514350"/>
+          <a:ext cx="1332000" cy="432000"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip1Rect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 47535"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="72000" rIns="36000" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1000">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+            </a:rPr>
+            <a:t>LANÇAMENTOS</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>141375</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>60525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Retângulo: Único Canto Recortado 10">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F6DEA5C-FE02-4F70-AC4E-521F970DE373}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2962275" y="514350"/>
+          <a:ext cx="1332000" cy="432000"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip1Rect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 47535"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="72000" rIns="36000" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1000">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+            </a:rPr>
+            <a:t>RELATÓRIOS</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>560475</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>60525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo: Único Canto Recortado 7">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68D92666-11B7-401A-B465-5FF5EE91444B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="257175" y="514350"/>
+          <a:ext cx="1332000" cy="432000"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip1Rect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 47535"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="72000" rIns="36000" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1000">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+            </a:rPr>
+            <a:t>MENU</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142875</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>155113</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagem 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8DD455D8-DD2E-4E47-A793-02EFDF9CAC96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill rotWithShape="1">
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:srcRect t="4111" b="8450"/>
+        <a:stretch/>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4286250" y="1162050"/>
+          <a:ext cx="3133725" cy="2784013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>19050</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>314850</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>504000</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="CaixaDeTexto 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88F505DC-0525-4B37-B8DC-24B423530C24}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="266700" y="0"/>
+          <a:ext cx="3420000" cy="504000"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1500">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t>GERENCIADOR</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1500" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="bg1"/>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+            </a:rPr>
+            <a:t> DE ESTOQUES</a:t>
+          </a:r>
+          <a:endParaRPr lang="pt-BR" sz="1500">
+            <a:solidFill>
+              <a:schemeClr val="bg1"/>
+            </a:solidFill>
+            <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>581025</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>350925</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>60525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Retângulo: Único Canto Recortado 6">
+          <a:hlinkClick xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{61A5EA32-C5C9-47A5-A9FE-68ABE8608E4C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1609725" y="514350"/>
+          <a:ext cx="1332000" cy="432000"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip1Rect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 47535"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" lIns="72000" rIns="36000" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="1000">
+              <a:solidFill>
+                <a:schemeClr val="bg2">
+                  <a:lumMod val="50000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Arial Black" panose="020B0A04020102020204" pitchFamily="34" charset="0"/>
+              <a:cs typeface="Aharoni" panose="02010803020104030203" pitchFamily="2" charset="-79"/>
+            </a:rPr>
+            <a:t>LANÇAMENTOS</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>371475</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>141375</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>60525</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Retângulo: Único Canto Recortado 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8F6DEA5C-FE02-4F70-AC4E-521F970DE373}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2962275" y="514350"/>
+          <a:ext cx="1332000" cy="432000"/>
+        </a:xfrm>
+        <a:prstGeom prst="snip1Rect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 47535"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
         <a:ln>
           <a:noFill/>
         </a:ln>
@@ -875,7 +1624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1229,4 +1978,731 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q23"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="16" width="11.7109375" customWidth="1"/>
+    <col min="17" max="17" width="3.7109375" customWidth="1"/>
+    <col min="18" max="16384" width="11.7109375" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:16" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="11"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="13"/>
+    </row>
+    <row r="2" spans="2:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="16"/>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="4"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="7"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="7"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="7"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="7"/>
+    </row>
+    <row r="8" spans="2:16" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="B8" s="5"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="7"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="7"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="7"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="7"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="7"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="7"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="7"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="7"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="7"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="7"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="7"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="7"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="10"/>
+    </row>
+    <row r="23" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B23" t="s">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q20"/>
+  <sheetViews>
+    <sheetView showGridLines="0" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="3.7109375" customWidth="1"/>
+    <col min="2" max="16" width="11.7109375" customWidth="1"/>
+    <col min="17" max="17" width="3.7109375" customWidth="1"/>
+    <col min="18" max="16384" width="11.7109375" hidden="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:16" s="1" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="11"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="13"/>
+    </row>
+    <row r="2" spans="2:16" s="1" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="14"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
+      <c r="J2" s="15"/>
+      <c r="K2" s="15"/>
+      <c r="L2" s="15"/>
+      <c r="M2" s="15"/>
+      <c r="N2" s="15"/>
+      <c r="O2" s="15"/>
+      <c r="P2" s="16"/>
+    </row>
+    <row r="3" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B3" s="2"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="4"/>
+    </row>
+    <row r="4" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B4" s="5"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="7"/>
+    </row>
+    <row r="5" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B5" s="5"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="7"/>
+    </row>
+    <row r="6" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B6" s="5"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="7"/>
+    </row>
+    <row r="7" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B7" s="5"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="7"/>
+    </row>
+    <row r="8" spans="2:16" ht="18.75" x14ac:dyDescent="0.4">
+      <c r="B8" s="5"/>
+      <c r="C8" s="17"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="7"/>
+    </row>
+    <row r="9" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B9" s="5"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="7"/>
+    </row>
+    <row r="10" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B10" s="5"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="7"/>
+    </row>
+    <row r="11" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B11" s="5"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="7"/>
+    </row>
+    <row r="12" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B12" s="5"/>
+      <c r="C12" s="6"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
+      <c r="K12" s="6"/>
+      <c r="L12" s="6"/>
+      <c r="M12" s="6"/>
+      <c r="N12" s="6"/>
+      <c r="O12" s="6"/>
+      <c r="P12" s="7"/>
+    </row>
+    <row r="13" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B13" s="5"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="6"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
+      <c r="N13" s="6"/>
+      <c r="O13" s="6"/>
+      <c r="P13" s="7"/>
+    </row>
+    <row r="14" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B14" s="5"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
+      <c r="K14" s="6"/>
+      <c r="L14" s="6"/>
+      <c r="M14" s="6"/>
+      <c r="N14" s="6"/>
+      <c r="O14" s="6"/>
+      <c r="P14" s="7"/>
+    </row>
+    <row r="15" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B15" s="5"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="6"/>
+      <c r="M15" s="6"/>
+      <c r="N15" s="6"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="7"/>
+    </row>
+    <row r="16" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B16" s="5"/>
+      <c r="C16" s="6"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
+      <c r="K16" s="6"/>
+      <c r="L16" s="6"/>
+      <c r="M16" s="6"/>
+      <c r="N16" s="6"/>
+      <c r="O16" s="6"/>
+      <c r="P16" s="7"/>
+    </row>
+    <row r="17" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B17" s="5"/>
+      <c r="C17" s="6"/>
+      <c r="D17" s="6"/>
+      <c r="E17" s="6"/>
+      <c r="F17" s="6"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="6"/>
+      <c r="M17" s="6"/>
+      <c r="N17" s="6"/>
+      <c r="O17" s="6"/>
+      <c r="P17" s="7"/>
+    </row>
+    <row r="18" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B18" s="5"/>
+      <c r="C18" s="6"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="6"/>
+      <c r="M18" s="6"/>
+      <c r="N18" s="6"/>
+      <c r="O18" s="6"/>
+      <c r="P18" s="7"/>
+    </row>
+    <row r="19" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B19" s="5"/>
+      <c r="C19" s="6"/>
+      <c r="D19" s="6"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="6"/>
+      <c r="M19" s="6"/>
+      <c r="N19" s="6"/>
+      <c r="O19" s="6"/>
+      <c r="P19" s="7"/>
+    </row>
+    <row r="20" spans="2:16" x14ac:dyDescent="0.25">
+      <c r="B20" s="8"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="9"/>
+      <c r="O20" s="9"/>
+      <c r="P20" s="10"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>